<commit_message>
lekkage probleem, kga nr huis, vogel is doing great
</commit_message>
<xml_diff>
--- a/ProcurementList.xlsx
+++ b/ProcurementList.xlsx
@@ -546,7 +546,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -939,7 +939,7 @@
         <v>47</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>48</v>
@@ -952,7 +952,7 @@
       </c>
       <c r="G27" s="2" t="n">
         <f aca="false">F27*C27</f>
-        <v>30.9</v>
+        <v>47.38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,7 +967,7 @@
       </c>
       <c r="G28" s="2" t="n">
         <f aca="false">F28*C27</f>
-        <v>45.6</v>
+        <v>69.92</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +982,7 @@
       </c>
       <c r="G29" s="2" t="n">
         <f aca="false">F29*C27</f>
-        <v>15.6</v>
+        <v>23.92</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>18</v>
@@ -996,7 +996,7 @@
         <v>54</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>55</v>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="G32" s="2" t="n">
         <f aca="false">F32*C31</f>
-        <v>5.7</v>
+        <v>8.74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="G33" s="2" t="n">
         <f aca="false">F33*C31</f>
-        <v>3.6</v>
+        <v>5.52</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>18</v>
@@ -1055,7 +1055,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="G37" s="2" t="n">
         <f aca="false">F37*C35</f>
-        <v>176.56</v>
+        <v>88.28</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>18</v>
@@ -1081,7 +1081,7 @@
         <v>65</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,7 +1089,7 @@
         <v>66</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
at least made some progress on this front
</commit_message>
<xml_diff>
--- a/ProcurementList.xlsx
+++ b/ProcurementList.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
   <si>
     <t xml:space="preserve">Construction</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.tuli-shop.com/aluminium-profile-40x40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">*</t>
@@ -266,22 +263,95 @@
     <t xml:space="preserve">https://www.tuli-shop.com/flange-nut-m8</t>
   </si>
   <si>
+    <t xml:space="preserve">Leveling feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI Leveling feet M8 F150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/leveling-feet-fi50-m8</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ball Bearings</t>
   </si>
   <si>
-    <t xml:space="preserve">Z-Axis Floating Side Support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TULI BF 15 Economy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.tuli-shop.com/economy-ball-screw-support-bearing-bf-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-Axis Fixed side support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-Axis Ball screw shaft + nut </t>
+    <t xml:space="preserve">Y-Axis Fixed Side Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI BF12 Economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/economy-ball-screw-support-bearing-bf-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y-Axis Floating side support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI BK12 SYK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/syk-ball-screw-support-bearing-bk-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI BK12 Economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/economy-ball-screw-support-bearing-bk-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y-Axis Ball screw shaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCR 1604 F C5 TBI Motion
+, with BK12 and BF12 end matching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/tbi-motion-ball-screw-scr-1604-f-c5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y-Axis Ball screw nut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MGD 16 syk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/syk-ball-screw-nut-bracket-mgd-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y-Axis rail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI A25 ALULIN 400mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/alulin-linear-guide-rail-a25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y-Axis block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI GNS-2500 ALULIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/us/alulin-linear-block-gns-2500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10 M6 Hammer nuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI Hammer nut M6 U10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/us/hammer-nut-u10m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M6 L20 Cylindrical screws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULI Screw with cylindrical head M6 L20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tuli-shop.com/us/screw-cylindrical-head-m6l20</t>
   </si>
 </sst>
 </file>
@@ -390,7 +460,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -417,6 +487,14 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -543,10 +621,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F50" activeCellId="0" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -639,28 +717,29 @@
       <c r="F5" s="2" t="n">
         <v>32.08</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>17</v>
+      <c r="G5" s="2" t="n">
+        <f aca="false">F5*C3</f>
+        <v>128.32</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>10.76</v>
@@ -672,7 +751,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>14</v>
@@ -687,7 +766,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
@@ -700,24 +779,24 @@
         <v>25.92</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>8.05</v>
@@ -729,7 +808,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>14</v>
@@ -744,7 +823,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
@@ -757,24 +836,24 @@
         <v>16.16</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>75.34</v>
@@ -786,7 +865,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>14</v>
@@ -801,7 +880,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
@@ -814,24 +893,24 @@
         <v>174.36</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>31.23</v>
@@ -843,10 +922,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>44.67</v>
@@ -858,10 +937,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>24.95</v>
@@ -871,24 +950,24 @@
         <v>99.8</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>5.44</v>
@@ -900,10 +979,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>5.41</v>
@@ -915,10 +994,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>1.56</v>
@@ -928,81 +1007,81 @@
         <v>37.44</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>1.03</v>
       </c>
       <c r="G27" s="2" t="n">
         <f aca="false">F27*C27</f>
-        <v>47.38</v>
+        <v>30.9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>1.52</v>
       </c>
       <c r="G28" s="2" t="n">
         <f aca="false">F28*C27</f>
-        <v>69.92</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0.52</v>
       </c>
       <c r="G29" s="2" t="n">
         <f aca="false">F29*C27</f>
-        <v>23.92</v>
+        <v>15.6</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>68.97</v>
@@ -1013,83 +1092,290 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0.19</v>
       </c>
       <c r="G32" s="2" t="n">
         <f aca="false">F32*C31</f>
-        <v>8.74</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="F33" s="2" t="n">
         <v>0.12</v>
       </c>
       <c r="G33" s="2" t="n">
         <f aca="false">F33*C31</f>
-        <v>5.52</v>
+        <v>3.6</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>44.14</v>
+        <v>3.62</v>
       </c>
       <c r="G37" s="2" t="n">
         <f aca="false">F37*C35</f>
-        <v>88.28</v>
+        <v>14.48</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="B39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>2</v>
       </c>
     </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>29.75</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <f aca="false">C39*F41</f>
+        <v>59.5</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>71.98</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <f aca="false">C43*F44</f>
+        <v>143.96</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>59.22</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <f aca="false">F45*C43</f>
+        <v>118.44</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <v>114.33</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <f aca="false">F49*C47</f>
+        <v>228.66</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F53" s="2" t="n">
+        <v>47.32</v>
+      </c>
+      <c r="G53" s="2" t="n">
+        <f aca="false">F53*C51</f>
+        <v>94.64</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>40.88</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <f aca="false">C55*F57</f>
+        <v>163.52</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F61" s="2" t="n">
+        <v>62.15</v>
+      </c>
+      <c r="G61" s="2" t="n">
+        <f aca="false">C59*F61</f>
+        <v>248.6</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F65" s="2" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <f aca="false">C63*F65</f>
+        <v>14</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D69" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F69" s="2" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G69" s="2" t="n">
+        <f aca="false">F69*C67</f>
+        <v>4.8</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1116,13 +1402,19 @@
     <hyperlink ref="E31" r:id="rId20" display="https://us.misumi-ec.com/vona2/detail/221000544985/?Tab=wysiwyg_area_0&amp;curSearch=%7b%22field%22%3a%22%40search%22%2c%22seriesCode%22%3a%22221000544985%22%2c%22innerCode%22%3a%22%22%2c%22sort%22%3a1%2c%22specSortFlag%22%3a0%2c%22allSpecFlag%22%3a0%2c%22page%22%3a1%2c%22pageSize%22%3a%2260%22%2c%2200000070744%22%3a%22mig00000001420512%22%2c%2200000069967%22%3a%2200000069967.a!00201%22%2c%2200000071933%22%3a%22d%22%2c%2200000071976%22%3a%2200000071976.f!00052%22%2c%22fixedInfo%22%3a%22innerCode%3aMDM00005884393%7c10%22%7d"/>
     <hyperlink ref="E32" r:id="rId21" display="https://parco-inc.com/product/m6-flanged-hex-nut-bright-zinc/"/>
     <hyperlink ref="E33" r:id="rId22" display="https://www.tuli-shop.com/flange-nut-m8"/>
+    <hyperlink ref="E41" r:id="rId23" display="https://www.tuli-shop.com/economy-ball-screw-support-bearing-bf-12"/>
+    <hyperlink ref="E44" r:id="rId24" display="https://www.tuli-shop.com/syk-ball-screw-support-bearing-bk-12"/>
+    <hyperlink ref="E45" r:id="rId25" display="https://www.tuli-shop.com/economy-ball-screw-support-bearing-bk-12"/>
+    <hyperlink ref="E49" r:id="rId26" display="https://www.tuli-shop.com/tbi-motion-ball-screw-scr-1604-f-c5"/>
+    <hyperlink ref="E53" r:id="rId27" display="https://www.tuli-shop.com/syk-ball-screw-nut-bracket-mgd-16"/>
+    <hyperlink ref="E57" r:id="rId28" display="https://www.tuli-shop.com/alulin-linear-guide-rail-a25"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>